<commit_message>
add automatics proofs and fix some bugs
</commit_message>
<xml_diff>
--- a/Doc/reports/algorithms complexity.xlsx
+++ b/Doc/reports/algorithms complexity.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhonatan\Desktop\Laboratory-1\Doc\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3EA6380B-67ED-4D63-B581-7A10476BCD3A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{10FE499A-358D-4670-8BA5-23D305532611}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="1" activeTab="1" xr2:uid="{F0253F08-5E33-4A01-AEFD-E68A3903E141}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="2" xr2:uid="{F0253F08-5E33-4A01-AEFD-E68A3903E141}"/>
   </bookViews>
   <sheets>
     <sheet name="PigeonHoleSort" sheetId="1" r:id="rId1"/>
     <sheet name="RadixSort" sheetId="2" r:id="rId2"/>
+    <sheet name="QuickSort" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="105">
   <si>
     <t>public static void pigeonhole_sort(int arr[],int n)</t>
   </si>
@@ -886,6 +887,81 @@
       </rPr>
       <t>(bitTemp &gt; mx)</t>
     </r>
+  </si>
+  <si>
+    <t>public void quickSort(int[] list, int high, int low ) {</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     quickSort(list,partition+1,high);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                      int partition = partition(list,low,high);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             if(low&lt;high)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     quickSort(list,low, partition-1);</t>
+  </si>
+  <si>
+    <t>Temporal</t>
+  </si>
+  <si>
+    <t>private int partition(int[] list, int low, int high) {</t>
+  </si>
+  <si>
+    <t>int pivot = list[high];</t>
+  </si>
+  <si>
+    <t>int smallerElementIndex = (low-1);</t>
+  </si>
+  <si>
+    <t>for (int i = low; i &lt; high; i++) {</t>
+  </si>
+  <si>
+    <t>if(list[i]&lt;=pivot)</t>
+  </si>
+  <si>
+    <t>int temp = list[smallerElementIndex+1];</t>
+  </si>
+  <si>
+    <t>list[smallerElementIndex+1] = list[high];</t>
+  </si>
+  <si>
+    <t>list[high] = temp;</t>
+  </si>
+  <si>
+    <t>return smallerElementIndex+1;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            list[i] = temp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            int temp = list[smallerElementIndex];</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            list[smallerElementIndex] = list[i];</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            smallerElementIndex++;</t>
+  </si>
+  <si>
+    <t>n-2</t>
+  </si>
+  <si>
+    <t>T(n) = [(n-1)n]/2</t>
   </si>
 </sst>
 </file>
@@ -1446,7 +1522,7 @@
   <dimension ref="B2:D36"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1718,7 +1794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A01B6971-0C6A-4602-828B-69ECC28FEB71}">
   <dimension ref="A2:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I13" workbookViewId="0">
+    <sheetView topLeftCell="I13" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -2172,4 +2248,197 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13782C92-C5C5-4BB5-978D-1DB2DAF1190C}">
+  <dimension ref="B1:H27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8">
+      <c r="C1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8">
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="F7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="F11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="F14" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="F16" t="s">
+        <v>99</v>
+      </c>
+      <c r="G16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="6:7">
+      <c r="F18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="6:7">
+      <c r="F19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="6:7">
+      <c r="F22" t="s">
+        <v>94</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="6:7">
+      <c r="F23" t="s">
+        <v>95</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="6:7">
+      <c r="F24" t="s">
+        <v>96</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="6:7">
+      <c r="F26" t="s">
+        <v>97</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="6:7">
+      <c r="F27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>